<commit_message>
updated AB and function
</commit_message>
<xml_diff>
--- a/api/Model/Python file for Cartofact data extracting/at_table.xlsx
+++ b/api/Model/Python file for Cartofact data extracting/at_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -368,256 +368,43 @@
           <t>table</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>search_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>licence</t>
+          <t>field_name</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>live_well_ab</t>
+          <t>live_well_ab_st98_field_oil_reserve</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>field_name</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>uwi_formatted</t>
+          <t>oil_in_place_e3m3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>spud_date</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>cumulative_oil_production_m3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>cumulative_gas_production_e3m3</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>cumulative_water_production_m3</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>cumulative_condensate_production_bbl</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>completion_interval_bottom</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>prod_ip3_oil_bbld</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>prod_ip3_gas_mcfd</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ground_elevation</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>status_full</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>llr_abandonment_area_name</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>surf_aband_date</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>tv_depth</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>well_total_depth</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+          <t>live_well_ab_st98_field_oil_reserve</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>field_name</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>last_production_date</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>prod_ip3_boe_boed</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>prod_mr3_wtr_bbld</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>prod_mr3_oil_bbld</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>live_well_ab</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
r code paths changed
</commit_message>
<xml_diff>
--- a/api/Model/Python file for Cartofact data extracting/at_table.xlsx
+++ b/api/Model/Python file for Cartofact data extracting/at_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -368,43 +368,220 @@
           <t>table</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>search_id</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>field_name</t>
+          <t>well_authority_number</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>live_well_ab_st98_field_oil_reserve</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>field_name</t>
+          <t>live_well_bc</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>oil_in_place_e3m3</t>
+          <t>uwi_formatted</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>live_well_ab_st98_field_oil_reserve</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>field_name</t>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>geom</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>spud_date</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>cumulative_oil_production_m3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>cumulative_gas_production_e3m3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>cumulative_water_production_m3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>cumulative_condensate_production_bbl</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>completion_bottom_depth_m</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>prod_ip3_oil_bbld</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>prod_ip3_gas_mcfd</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>full_status</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>total_drilled_depth_m</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>last_production_date</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>prod_ip3_boe_boed</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>prod_mr3_wtr_bbld</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>prod_mr3_oil_bbld</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>cumulative_marketable_gas_production_mcf</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>live_well_bc</t>
         </is>
       </c>
     </row>

</xml_diff>